<commit_message>
add a foo on angr
</commit_message>
<xml_diff>
--- a/result_7_2_2.xlsx
+++ b/result_7_2_2.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WuhuangYao\Desktop\MTSan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wuhuangyao/MTSan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE85EC6-22DA-4D02-AAED-20CFED22F349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67BFF96-3130-0844-98BF-0D42621699AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25820" windowHeight="15240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
   <si>
     <t>CWE-ID</t>
   </si>
@@ -125,12 +124,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -145,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,9 +179,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -436,52 +474,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:Q11"/>
+  <dimension ref="A2:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.7265625" customWidth="1"/>
-    <col min="4" max="11" width="7.81640625" customWidth="1"/>
-    <col min="12" max="12" width="12.453125" customWidth="1"/>
-    <col min="13" max="14" width="7.81640625" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" customWidth="1"/>
-    <col min="16" max="17" width="7.81640625" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="5" width="7.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" customWidth="1"/>
+    <col min="8" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="11" width="7.83203125" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="13" max="14" width="7.83203125" customWidth="1"/>
+    <col min="15" max="15" width="12.5" customWidth="1"/>
+    <col min="16" max="17" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>121</v>
       </c>
@@ -587,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>122</v>
       </c>
@@ -597,25 +639,25 @@
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="8">
         <v>3.7199999999999997E-2</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="5">
         <v>8.6800000000000002E-2</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="7">
         <v>5.2499999999999998E-2</v>
       </c>
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="6">
         <v>0.19689999999999999</v>
       </c>
       <c r="K5" s="1">
@@ -624,7 +666,7 @@
       <c r="L5" s="2">
         <v>0</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="6">
         <v>0.19689999999999999</v>
       </c>
       <c r="N5" s="1">
@@ -633,14 +675,14 @@
       <c r="O5" s="2">
         <v>0</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="6">
         <v>0.19689999999999999</v>
       </c>
       <c r="Q5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>124</v>
       </c>
@@ -693,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>126</v>
       </c>
@@ -746,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>127</v>
       </c>
@@ -799,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>415</v>
       </c>
@@ -852,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>416</v>
       </c>
@@ -905,7 +947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -954,6 +996,265 @@
       </c>
       <c r="Q11" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>121</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0.54290000000000005</v>
+      </c>
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.90190000000000003</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.44650000000000001</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0.44650000000000001</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.44650000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>122</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="8">
+        <v>3.7199999999999997E-2</v>
+      </c>
+      <c r="E16" s="5">
+        <v>8.6800000000000002E-2</v>
+      </c>
+      <c r="F16" s="7">
+        <v>5.2499999999999998E-2</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.19689999999999999</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.19689999999999999</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0.19689999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>124</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.27310000000000001</v>
+      </c>
+      <c r="E17" s="6">
+        <v>0.27739999999999998</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.2697</v>
+      </c>
+      <c r="G17" s="8">
+        <v>1.46E-2</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1.46E-2</v>
+      </c>
+      <c r="I17" s="8">
+        <v>1.46E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>126</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="7">
+        <v>0.6069</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="H18" s="8">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.53100000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>127</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.54879999999999995</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.3836</v>
+      </c>
+      <c r="F19" s="7">
+        <v>0.3836</v>
+      </c>
+      <c r="G19" s="8">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="H19" s="8">
+        <v>9.8500000000000004E-2</v>
+      </c>
+      <c r="I19" s="8">
+        <v>9.8500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>415</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>416</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="7">
+        <v>5.0900000000000001E-2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.1578</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.29010000000000002</v>
+      </c>
+      <c r="G21" s="8">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="H21" s="8">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="I21" s="8">
+        <v>3.0499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="7">
+        <v>0.29289999999999999</v>
+      </c>
+      <c r="E22" s="6">
+        <v>0.42609999999999998</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.39150000000000001</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.2417</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0.2417</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.2417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>